<commit_message>
fixing 2D x, y weirdness
</commit_message>
<xml_diff>
--- a/2D Euler/Speeding up Python.xlsx
+++ b/2D Euler/Speeding up Python.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pulsar/Documents/MSU/CA_CFD/2D Euler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321A401D-4E45-E744-9C73-1C1E5CF07329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F1EBC2-AEB1-E54C-8671-AB784A7F21B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00ADC960-4800-E342-BCEB-7005C541E381}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Comments</t>
   </si>
@@ -50,7 +50,16 @@
     <t>Initial run, not using jit at all. 32x32 grid, CFL = 0.1, t1 = 0.3, case = 0</t>
   </si>
   <si>
-    <t>adding @njit to the boundary condition function</t>
+    <t>adding @njit to the boundary_conditions function</t>
+  </si>
+  <si>
+    <t>removing @njit from the boundary_conditions function, removing cons2prim in w_half and get_flux, and adding @njit to w_half, get_flux, right_eigenvectors, and left_eigenvectors</t>
+  </si>
+  <si>
+    <t>adding @njit to weno and lf_flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 128x128 grid, CFL = 0.1, t1 = 0.3, case = 0</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -557,28 +566,42 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3">
+        <f>(123.54788+125.00538+115.54499)/3</f>
+        <v>121.36608333333334</v>
+      </c>
       <c r="B4" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>2.0227680555555554</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3">
+        <f>(12.31002+12.6224+13.26979)/3</f>
+        <v>12.734070000000001</v>
+      </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>0.21223450000000002</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3">
+        <v>468.19565</v>
+      </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>7.8032608333333338</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>

</xml_diff>